<commit_message>
refactoring for N vs N mode
</commit_message>
<xml_diff>
--- a/config_gen/config_chesstactic.xlsx
+++ b/config_gen/config_chesstactic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daejung/work/unity/Lemmings/Assets/Script/AI/config_gen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D053643-0668-6E44-B563-EE736D5E0603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E803619-455B-4245-A475-42B567A8718E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" xr2:uid="{2C1665BA-8C4D-8241-9A75-ACFF74886D12}"/>
   </bookViews>
@@ -37,12 +37,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="37">
   <si>
     <t>side</t>
-  </si>
-  <si>
-    <t>my</t>
   </si>
   <si>
     <t>id</t>
@@ -82,9 +79,6 @@
   </si>
   <si>
     <t>3,0,0</t>
-  </si>
-  <si>
-    <t>opp</t>
   </si>
   <si>
     <t>movingType
@@ -165,6 +159,12 @@
   "avoidance": 0.7,
   "retreat": 0.8
 }</t>
+  </si>
+  <si>
+    <t>내팀</t>
+  </si>
+  <si>
+    <t>적1</t>
   </si>
 </sst>
 </file>
@@ -545,8 +545,8 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -561,298 +561,298 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="187" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="187" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E2" s="2">
         <v>0</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="187" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="187" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" s="2">
         <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="187" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>1</v>
+      <c r="A4" s="2">
+        <v>0</v>
       </c>
       <c r="B4" s="2">
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" s="2">
         <v>2</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="187" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>1</v>
+      <c r="A5" s="2">
+        <v>0</v>
       </c>
       <c r="B5" s="2">
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" s="2">
         <v>0</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="187" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>1</v>
+      <c r="A6" s="2">
+        <v>0</v>
       </c>
       <c r="B6" s="2">
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E6" s="2">
         <v>0</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="187" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>1</v>
+      <c r="A7" s="2">
+        <v>0</v>
       </c>
       <c r="B7" s="2">
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E7" s="2">
         <v>2</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="187" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="2">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="2">
-        <v>0</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E8" s="2">
         <v>0</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="187" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>14</v>
+      <c r="A9" s="2">
+        <v>1</v>
       </c>
       <c r="B9" s="2">
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E9" s="2">
         <v>1</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="187" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>14</v>
+      <c r="A10" s="2">
+        <v>1</v>
       </c>
       <c r="B10" s="2">
         <v>2</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E10" s="2">
         <v>2</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="187" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>14</v>
+      <c r="A11" s="2">
+        <v>1</v>
       </c>
       <c r="B11" s="2">
         <v>3</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E11" s="2">
         <v>0</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="187" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>14</v>
+      <c r="A12" s="2">
+        <v>1</v>
       </c>
       <c r="B12" s="2">
         <v>4</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E12" s="2">
         <v>1</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="187" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>14</v>
+      <c r="A13" s="2">
+        <v>1</v>
       </c>
       <c r="B13" s="2">
         <v>5</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E13" s="2">
         <v>2</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -863,44 +863,53 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E4E66D8-4E1C-0141-8E34-4F0F28D831EC}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
       </c>
       <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
         <v>0</v>
       </c>
     </row>

</xml_diff>